<commit_message>
merge results with previous study
</commit_message>
<xml_diff>
--- a/Bayesian-Poker/experiment-results/2M-split/results-clean.xlsx
+++ b/Bayesian-Poker/experiment-results/2M-split/results-clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanjoneri/Projects/SURP-repos/SURP-2018/Bayesian-Poker/experiment-results/2M-split/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87179316-2CA5-704B-B8CE-C5C318582CAE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19B2CB2-61A4-6745-84E9-811DD41B4AE4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1880" windowWidth="28820" windowHeight="20940" activeTab="4" xr2:uid="{0F9F7D4F-EA70-EF43-B409-E1CF0DAF6D9F}"/>
+    <workbookView xWindow="1820" yWindow="1880" windowWidth="20160" windowHeight="20940" firstSheet="3" activeTab="11" xr2:uid="{0F9F7D4F-EA70-EF43-B409-E1CF0DAF6D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Round" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="BPP_final" sheetId="6" r:id="rId5"/>
     <sheet name="OPP_final" sheetId="7" r:id="rId6"/>
     <sheet name="BPP_win" sheetId="8" r:id="rId7"/>
-    <sheet name="Meta" sheetId="1" r:id="rId8"/>
+    <sheet name="Confidence" sheetId="9" r:id="rId8"/>
+    <sheet name="Joy" sheetId="10" r:id="rId9"/>
+    <sheet name="Anger" sheetId="11" r:id="rId10"/>
+    <sheet name="Surprise" sheetId="12" r:id="rId11"/>
+    <sheet name="Sorrow" sheetId="13" r:id="rId12"/>
+    <sheet name="Meta" sheetId="1" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="6">
   <si>
     <t>BPP_final</t>
   </si>
@@ -47,6 +52,9 @@
   </si>
   <si>
     <t>OPP_current</t>
+  </si>
+  <si>
+    <t>Confidence</t>
   </si>
 </sst>
 </file>
@@ -439,6 +447,379 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C5C39D-93DD-414C-AE16-285B3D67A7D1}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F82E72-CB0E-0A4C-BC6E-AC6D882C5EA9}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.4</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88486131-7E63-5040-A2A2-AD3C8EA2210A}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.7</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096B5786-E5C1-8045-A1EC-0E60EF7C76C3}">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>11</v>
+      </c>
+      <c r="D1">
+        <v>12</v>
+      </c>
+      <c r="E1">
+        <v>13</v>
+      </c>
+      <c r="F1">
+        <v>14</v>
+      </c>
+      <c r="G1">
+        <v>15</v>
+      </c>
+      <c r="H1">
+        <v>16</v>
+      </c>
+      <c r="I1">
+        <v>17</v>
+      </c>
+      <c r="J1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+      <c r="L1">
+        <v>4</v>
+      </c>
+      <c r="M1">
+        <v>5</v>
+      </c>
+      <c r="N1">
+        <v>6</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCF976F-1241-E44C-98B1-7EBCD46F0069}">
   <dimension ref="A1:S69"/>
@@ -12701,7 +13082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20DD5F6-77CE-0449-B1FA-DCF7B46662BB}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -13845,7 +14226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91781B21-E0DA-4B43-B181-5E39C5F6ED4A}">
   <dimension ref="A1:D290"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -18464,146 +18845,104 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096B5786-E5C1-8045-A1EC-0E60EF7C76C3}">
-  <dimension ref="A1:Q17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89FF94A-6B1B-C14C-884F-E1EBA0B003B7}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A701D98E-66AE-8641-9350-F917644F7A83}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F1">
-        <v>14</v>
-      </c>
-      <c r="G1">
-        <v>15</v>
-      </c>
-      <c r="H1">
-        <v>16</v>
-      </c>
-      <c r="I1">
-        <v>17</v>
-      </c>
-      <c r="J1">
-        <v>2</v>
-      </c>
-      <c r="K1">
-        <v>3</v>
-      </c>
-      <c r="L1">
-        <v>4</v>
-      </c>
-      <c r="M1">
         <v>5</v>
       </c>
-      <c r="N1">
-        <v>6</v>
-      </c>
-      <c r="O1">
-        <v>7</v>
-      </c>
-      <c r="P1">
-        <v>8</v>
-      </c>
-      <c r="Q1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>